<commit_message>
Revert "Auswertung der Umfrage"
This reverts commit 043237a325a31cc9bee7a397745423b22e542515.
</commit_message>
<xml_diff>
--- a/spezifikation/Umfrage_Auswertung.xlsx
+++ b/spezifikation/Umfrage_Auswertung.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -283,6 +283,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -308,7 +309,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -376,13 +377,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8</c:v>
@@ -390,11 +391,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9AFC-45D8-BB7E-F0AE6180DE73}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -450,7 +446,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="414743616"/>
@@ -508,7 +504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="414743224"/>
@@ -549,7 +545,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -561,7 +557,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -575,6 +571,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -600,7 +597,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -638,11 +635,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -658,11 +650,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -678,11 +665,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -698,11 +680,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -718,11 +695,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -740,11 +712,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -779,31 +746,26 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-209B-4FFC-A4C5-4D28F6B79E6E}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -826,6 +788,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -851,7 +814,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -881,7 +844,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -893,7 +856,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -934,6 +897,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -959,7 +923,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1001,16 +965,11 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9F3C-46BB-B196-2B37D33C38BF}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1048,11 +1007,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9F3C-46BB-B196-2B37D33C38BF}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1133,7 +1087,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="483661392"/>
@@ -1150,6 +1104,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1175,7 +1130,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1205,7 +1160,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1217,7 +1172,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1231,6 +1186,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1256,7 +1212,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1304,11 +1260,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-F1CC-4761-B24F-7E386CAF5907}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1323,11 +1274,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-F1CC-4761-B24F-7E386CAF5907}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1342,11 +1288,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-F1CC-4761-B24F-7E386CAF5907}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1389,11 +1330,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F1CC-4761-B24F-7E386CAF5907}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1449,7 +1385,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="489851064"/>
@@ -1507,7 +1443,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="489849888"/>
@@ -1548,7 +1484,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1560,7 +1496,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1574,6 +1510,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1599,7 +1536,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1636,11 +1573,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-C9B0-4FC5-8967-D0ED97BE73C3}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1656,11 +1588,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-C9B0-4FC5-8967-D0ED97BE73C3}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1677,11 +1604,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-C9B0-4FC5-8967-D0ED97BE73C3}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1707,22 +1629,17 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-C9B0-4FC5-8967-D0ED97BE73C3}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1745,6 +1662,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1770,7 +1688,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1800,7 +1718,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1812,7 +1730,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1826,6 +1744,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1851,7 +1770,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1916,28 +1835,23 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C910-471F-947B-97BAA296415A}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1993,7 +1907,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="483681192"/>
@@ -2051,7 +1965,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="483680800"/>
@@ -2092,7 +2006,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2104,7 +2018,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -2118,6 +2032,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2143,7 +2058,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2205,10 +2120,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -2219,11 +2134,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-65AB-4584-848C-376CF077D4A7}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2279,7 +2189,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="489229856"/>
@@ -2337,7 +2247,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="489227896"/>
@@ -2378,7 +2288,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2390,7 +2300,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -2441,6 +2351,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2466,7 +2377,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2508,16 +2419,11 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-47B7-49E7-B3C5-EEAD6F805CE8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2550,16 +2456,11 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-47B7-49E7-B3C5-EEAD6F805CE8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2640,7 +2541,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="493425896"/>
@@ -2657,6 +2558,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2682,7 +2584,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2712,7 +2614,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2724,7 +2626,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -2772,6 +2674,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2797,7 +2700,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2839,16 +2742,11 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7DB3-4078-8767-62E0B6C6F3C4}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2881,16 +2779,11 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7DB3-4078-8767-62E0B6C6F3C4}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2971,7 +2864,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="487527400"/>
@@ -2988,6 +2881,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3013,7 +2907,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3043,7 +2937,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7996,13 +7890,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagramm 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8032,13 +7920,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8068,13 +7950,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagramm 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Diagramm 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8104,13 +7980,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Diagramm 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="7" name="Diagramm 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8140,13 +8010,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Diagramm 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="8" name="Diagramm 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8176,13 +8040,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Diagramm 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="9" name="Diagramm 8"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8212,13 +8070,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Diagramm 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="10" name="Diagramm 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8248,13 +8100,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Diagramm 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="11" name="Diagramm 10"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8284,13 +8130,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Diagramm 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="12" name="Diagramm 11"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8309,7 +8149,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -8384,23 +8224,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8436,23 +8259,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8607,14 +8413,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="N84" sqref="N84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" style="1"/>
-    <col min="2" max="2" width="3.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.88671875" style="1"/>
     <col min="5" max="5" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.88671875" style="1"/>
@@ -8644,7 +8450,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
@@ -8652,7 +8458,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -8660,7 +8466,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
@@ -8687,7 +8493,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -8695,7 +8501,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -8703,7 +8509,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
@@ -8711,7 +8517,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -8719,7 +8525,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
@@ -8727,7 +8533,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -8746,7 +8552,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -8813,7 +8619,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="3">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>20</v>
@@ -8821,7 +8627,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>22</v>
@@ -8829,7 +8635,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="3">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>21</v>
@@ -8848,7 +8654,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="3">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>25</v>
@@ -8864,7 +8670,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>27</v>
@@ -8872,7 +8678,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>41</v>
@@ -8880,7 +8686,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>42</v>
@@ -8896,7 +8702,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B50" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>29</v>
@@ -8904,7 +8710,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B51" s="3">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>43</v>
@@ -8939,7 +8745,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B57" s="3">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>31</v>
@@ -8947,7 +8753,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B58" s="3">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>32</v>
@@ -8963,7 +8769,7 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B62" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>14</v>
@@ -8971,7 +8777,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B63" s="3">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>32</v>

</xml_diff>